<commit_message>
tidied up some stuff and finished some other stuff. Reran the top10 things with the fixed data.txt
</commit_message>
<xml_diff>
--- a/TBDF_MeanVariance_FirstVersion.xlsx
+++ b/TBDF_MeanVariance_FirstVersion.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Studium\AA_Courses\Semester_4\Project\AE2223-I-Group-CD9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{02354DEF-049A-4460-BA10-E6CBA84BD9BA}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F432BAF1-69B8-46D5-ADB0-91B582D4647F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TBDF_MeanVariance_FirstVersion" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2792,11 +2792,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>